<commit_message>
Almost finished the tableMapping
</commit_message>
<xml_diff>
--- a/DOCS/Drafts/Design Spec/TableMapping.xlsx
+++ b/DOCS/Drafts/Design Spec/TableMapping.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="15315" windowHeight="8760"/>
+    <workbookView xWindow="16820" yWindow="5380" windowWidth="8000" windowHeight="7720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Requirement</t>
   </si>
@@ -60,7 +65,16 @@
     <t>CommunicationClass, LinkInterface</t>
   </si>
   <si>
-    <t>LocationClass,KeyLocationClass</t>
+    <t>WalkActivityClass</t>
+  </si>
+  <si>
+    <t>TourClass, WalkActivityClass</t>
+  </si>
+  <si>
+    <t>MainActivityClass</t>
+  </si>
+  <si>
+    <t>KeyLocationClass, LocationClass</t>
   </si>
 </sst>
 </file>
@@ -100,16 +114,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -117,11 +131,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,90 +447,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -517,6 +539,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -526,9 +553,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -538,8 +570,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>